<commit_message>
Updated acceptance testing report.
</commit_message>
<xml_diff>
--- a/static/docs/peppol/aptest.xlsx
+++ b/static/docs/peppol/aptest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebe\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebe\IdeaProjects\vefa-portal\static\docs\peppol\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5PshQgIYZUm8oMXpyXqINOyAnqEiP9TmA63PYTKCxezAAPyiyz35LA/yemjzdPCMgOsgdLlWRgeD/rU9C6YO2g==" workbookSaltValue="6KAR8qyXW3qOdFTn3AMhsw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -111,9 +111,6 @@
     <t>Transfer error while sending a document</t>
   </si>
   <si>
-    <t>Activities to make sure certificate is valid</t>
-  </si>
-  <si>
     <t>Describe your routines for the following situations:</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Tester</t>
+  </si>
+  <si>
+    <t>Activities to make sure your certificate is valid</t>
   </si>
 </sst>
 </file>
@@ -191,13 +191,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,15 +571,15 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -613,13 +613,13 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -627,13 +627,13 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -667,13 +667,13 @@
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -681,10 +681,10 @@
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -695,10 +695,10 @@
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -735,13 +735,13 @@
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -749,10 +749,10 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -820,12 +820,12 @@
         <v>13</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -834,12 +834,12 @@
         <v>14</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -874,12 +874,12 @@
         <v>16</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -914,12 +914,12 @@
         <v>19</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -954,12 +954,12 @@
         <v>21</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -994,12 +994,12 @@
         <v>23</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1031,7 +1031,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1070,14 +1070,14 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -1108,14 +1108,14 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -1146,14 +1146,14 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -1171,7 +1171,7 @@
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1184,14 +1184,14 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -1207,8 +1207,10 @@
       <c r="J51" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GVz1RafbuNrgsj8eTTVGyG7ElWoyp8MoAsmvtUFPfilRy/xzA+i9NOtScK+v+siaenL+IJdQLNM/H1gNCFD6jw==" saltValue="+w++gZa/qe5uUOJzvquxrA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UoU+1OBrNYzKk+w8HR2oMSNetpC/9XnaFaQqTUvmJ3IqEa7ug6lto5gL0WnwHf1w9tE1e8T6Pcjm9834UYUkSw==" saltValue="LaxDeOxlTuSY9tMGryse5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
     <mergeCell ref="B50:I50"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="D22:H22"/>
@@ -1225,8 +1227,6 @@
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="D35:H35"/>
     <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update acceptance testing report.
</commit_message>
<xml_diff>
--- a/static/docs/peppol/aptest.xlsx
+++ b/static/docs/peppol/aptest.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5PshQgIYZUm8oMXpyXqINOyAnqEiP9TmA63PYTKCxezAAPyiyz35LA/yemjzdPCMgOsgdLlWRgeD/rU9C6YO2g==" workbookSaltValue="6KAR8qyXW3qOdFTn3AMhsw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -198,6 +198,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -517,16 +521,16 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:H22"/>
+      <selection activeCell="B41" sqref="B41:I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:10" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -540,7 +544,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -552,7 +556,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -566,7 +570,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -582,7 +586,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -594,7 +598,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -608,7 +612,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -622,7 +626,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
@@ -636,7 +640,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -648,7 +652,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>30</v>
@@ -662,7 +666,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -676,7 +680,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -690,7 +694,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -704,7 +708,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -716,7 +720,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -730,7 +734,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -744,7 +748,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -758,7 +762,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -770,7 +774,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>15</v>
@@ -784,7 +788,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -800,7 +804,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>10</v>
@@ -814,7 +818,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
@@ -828,7 +832,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -842,7 +846,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -854,7 +858,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -868,7 +872,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>16</v>
@@ -882,7 +886,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -894,7 +898,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>18</v>
@@ -908,7 +912,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>19</v>
@@ -922,7 +926,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -934,7 +938,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
         <v>20</v>
@@ -948,7 +952,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
@@ -962,7 +966,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -974,7 +978,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>22</v>
@@ -988,7 +992,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>23</v>
@@ -1002,7 +1006,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1014,7 +1018,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="3" t="s">
         <v>24</v>
@@ -1028,7 +1032,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>28</v>
@@ -1042,7 +1046,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1054,7 +1058,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>25</v>
@@ -1068,19 +1072,19 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1092,7 +1096,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>26</v>
@@ -1106,19 +1110,19 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1130,7 +1134,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>27</v>
@@ -1144,19 +1148,19 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1168,7 +1172,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>31</v>
@@ -1182,19 +1186,19 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1207,8 +1211,10 @@
       <c r="J51" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UoU+1OBrNYzKk+w8HR2oMSNetpC/9XnaFaQqTUvmJ3IqEa7ug6lto5gL0WnwHf1w9tE1e8T6Pcjm9834UYUkSw==" saltValue="LaxDeOxlTuSY9tMGryse5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="w6Wy1jbg8FuAl8fqYZpfxHVR21jHefAHjRgc5v++RzqICouVxZWSAm4i09f4alJH/LKPRI5gaomD7tWWKSssug==" saltValue="74cMXWb18HOAqS+T9d9yLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="B41:I41"/>
     <mergeCell ref="B44:I44"/>
     <mergeCell ref="B47:I47"/>
     <mergeCell ref="B50:I50"/>
@@ -1225,8 +1231,6 @@
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="B41:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Clarifications related to acceptance testing.
</commit_message>
<xml_diff>
--- a/static/docs/peppol/aptest.xlsx
+++ b/static/docs/peppol/aptest.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5PshQgIYZUm8oMXpyXqINOyAnqEiP9TmA63PYTKCxezAAPyiyz35LA/yemjzdPCMgOsgdLlWRgeD/rU9C6YO2g==" workbookSaltValue="6KAR8qyXW3qOdFTn3AMhsw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>Tester</t>
   </si>
   <si>
-    <t>Activities to make sure your certificate is valid</t>
+    <t>Activities to make sure your PEPPOL certificate is continuous valid</t>
   </si>
 </sst>
 </file>
@@ -198,10 +198,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -520,17 +520,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:I41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -544,7 +544,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -556,7 +556,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -570,7 +570,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -586,7 +586,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -598,7 +598,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -612,35 +612,35 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -652,7 +652,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>30</v>
@@ -666,7 +666,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -680,7 +680,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -694,7 +694,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -708,7 +708,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -720,7 +720,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>5</v>
@@ -734,7 +734,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -748,7 +748,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -762,7 +762,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -774,7 +774,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
         <v>15</v>
@@ -788,7 +788,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -804,7 +804,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>10</v>
@@ -818,7 +818,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
@@ -832,7 +832,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -846,7 +846,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -858,7 +858,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -872,7 +872,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>16</v>
@@ -886,7 +886,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -898,7 +898,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>18</v>
@@ -912,7 +912,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>19</v>
@@ -926,7 +926,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -938,7 +938,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
         <v>20</v>
@@ -952,7 +952,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
@@ -966,7 +966,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -978,7 +978,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>22</v>
@@ -992,7 +992,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>23</v>
@@ -1006,7 +1006,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1018,7 +1018,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="1"/>
       <c r="B37" s="3" t="s">
         <v>24</v>
@@ -1032,7 +1032,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>28</v>
@@ -1046,7 +1046,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1058,7 +1058,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>25</v>
@@ -1072,19 +1072,19 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1096,7 +1096,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>26</v>
@@ -1110,19 +1110,19 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1134,7 +1134,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>27</v>
@@ -1148,19 +1148,19 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1172,7 +1172,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>31</v>
@@ -1186,19 +1186,19 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1211,18 +1211,9 @@
       <c r="J51" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="w6Wy1jbg8FuAl8fqYZpfxHVR21jHefAHjRgc5v++RzqICouVxZWSAm4i09f4alJH/LKPRI5gaomD7tWWKSssug==" saltValue="74cMXWb18HOAqS+T9d9yLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="a9TMG4TOBqg3FxflcW8XMG2xezAA2Oh5QH5gn4FxS6SW3ETtvRaOMl5YmYIngkfrZ6MI4HQh3vZFH0e2zKzFUw==" saltValue="C7FaMamWztKKaJGHoxY03Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D32:H32"/>
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="C11:I11"/>
@@ -1230,7 +1221,16 @@
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C17:F17"/>
-    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="B47:I47"/>
+    <mergeCell ref="B50:I50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>